<commit_message>
TestNG Repeat Day 2
</commit_message>
<xml_diff>
--- a/src/test/java/com/TestNG/Oct_01_2023_Day10_TestNG_ExcelSheet_DataProvider/ExcelData.xlsx
+++ b/src/test/java/com/TestNG/Oct_01_2023_Day10_TestNG_ExcelSheet_DataProvider/ExcelData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24A670A-316C-4DAB-8AF6-3C9D7A03DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA56BF-B496-4691-A375-DE20391DABAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginRediff" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginTN" sheetId="2" r:id="rId2"/>
-    <sheet name="RegisterTN" sheetId="3" r:id="rId3"/>
+    <sheet name="RegisterTN" sheetId="3" r:id="rId2"/>
+    <sheet name="LoginTN" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Shajlee1@</t>
   </si>
   <si>
-    <t>Mohamedboudguig@rediffmail.com</t>
-  </si>
-  <si>
-    <t>Medbgd0707@</t>
-  </si>
-  <si>
     <t>homa_rahimi@rediffmail.com</t>
   </si>
   <si>
@@ -86,35 +80,23 @@
     <t>seleniumpanda6@gmail.com</t>
   </si>
   <si>
-    <t>seleniumpanda7@gmail.com</t>
-  </si>
-  <si>
-    <t>seleniumpanda8@gmail.com</t>
-  </si>
-  <si>
-    <t>firsntame</t>
-  </si>
-  <si>
-    <t>Selenium</t>
+    <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
   </si>
   <si>
-    <t>Panda</t>
-  </si>
-  <si>
     <t>telephone</t>
   </si>
   <si>
-    <t>confirmpassword</t>
+    <t>email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,13 +151,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,12 +189,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,22 +217,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -529,18 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="93.1328125" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="93.15625" defaultRowHeight="18.3" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="16384" width="93.1328125" style="4"/>
+    <col min="1" max="16384" width="93.15625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -548,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -556,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -572,20 +544,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -596,31 +560,67 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{B05D47B7-41AD-4426-8EDF-27CE5C89CBA9}"/>
     <hyperlink ref="A4" r:id="rId5" xr:uid="{191355FE-E5FC-457D-BBE9-112A46B6080A}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{122654EB-54C5-4638-A777-92FE85D52354}"/>
-    <hyperlink ref="A5" r:id="rId7" xr:uid="{BB60C836-5A2F-4C71-AACA-CF6FDFE0A361}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{66BA37EA-E5C5-40EC-8183-EC5E6E380CFB}"/>
-    <hyperlink ref="A6" r:id="rId9" xr:uid="{A3C7608C-F304-4111-9F0B-8A4DF9FAF421}"/>
+    <hyperlink ref="A5" r:id="rId7" xr:uid="{A3C7608C-F304-4111-9F0B-8A4DF9FAF421}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2507C7-4AB5-4B65-9AA3-80CBD519A2BB}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A43442-C5E7-47B8-9D77-709CB5BBA45F}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30.75" x14ac:dyDescent="0.9"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="72.59765625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="61.3984375" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="7"/>
+    <col min="1" max="1" width="36.15625" customWidth="1"/>
+    <col min="2" max="2" width="29.68359375" customWidth="1"/>
+    <col min="3" max="3" width="35.9453125" customWidth="1"/>
+    <col min="4" max="4" width="36.62890625" customWidth="1"/>
+    <col min="5" max="5" width="29.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:5" ht="30.6" x14ac:dyDescent="1.1000000000000001">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2507C7-4AB5-4B65-9AA3-80CBD519A2BB}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="72.578125" customWidth="1"/>
+    <col min="2" max="2" width="61.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,75 +628,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="3" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="5" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="7" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.9">
+    <row r="8" spans="1:2" ht="30.6" x14ac:dyDescent="1.1000000000000001">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.9">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.9">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -711,204 +695,7 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{A87ACFD1-D6F6-496F-A359-28A659CDEAD7}"/>
     <hyperlink ref="B2" r:id="rId8" xr:uid="{BD2AA6D5-7C24-4DC0-BC1E-A82BC34EC867}"/>
     <hyperlink ref="B3:B8" r:id="rId9" display="Selenium@123" xr:uid="{D7247A02-2F0E-497E-805E-61EE56DDE543}"/>
-    <hyperlink ref="A10" r:id="rId10" xr:uid="{F813C678-C6DD-4C40-9BDF-7629603DAD0B}"/>
-    <hyperlink ref="B9" r:id="rId11" xr:uid="{177A3FE1-4295-4593-B3C2-1D15DF95F1B9}"/>
-    <hyperlink ref="B10" r:id="rId12" xr:uid="{CD6C7CD6-28CB-4430-89BC-DF1F42696723}"/>
-    <hyperlink ref="A9" r:id="rId13" xr:uid="{24B50BA3-FE78-4546-BA76-83D8AF5AEFE4}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE87A94-085A-4A26-A5FE-CC9318A22130}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="22.3984375" defaultRowHeight="30.75" x14ac:dyDescent="0.9"/>
-  <cols>
-    <col min="1" max="2" width="22.3984375" style="8"/>
-    <col min="3" max="3" width="32.53125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="30.59765625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="37.53125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="22.3984375" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="12">
-        <v>98765432</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>